<commit_message>
update document & Store Procedure
</commit_message>
<xml_diff>
--- a/Document/Bang_danh_gia.xlsx
+++ b/Document/Bang_danh_gia.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/University/He quan tri CSDL/untitled folder/BaoCao/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="32660" windowHeight="20540"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="32660" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +14,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>BẢNG ĐÁNH GIÁ CÁ NHÂN - NHÓM 5</t>
   </si>
@@ -87,39 +82,6 @@
   </si>
   <si>
     <t>Deadlock</t>
-  </si>
-  <si>
-    <t>Mô tả chức năng hệ thống
-Ràng buộc dữ liệu bổ sung
-Liệt kê mô tả ... lỗi tranh chấp (….)
-Tổng hợp báo cáo lần 1</t>
-  </si>
-  <si>
-    <t>Mô tả chức năng hệ thống
-Lược đồ kết hợp
-Ràng buộc dữ liệu bổ sung
-Liệt kê mô tả ... lỗi tranh chấp (….)
-Tổng hợp báo cáo lần 2</t>
-  </si>
-  <si>
-    <t>Mô tả chức năng hệ thống
-Ràng buộc dữ liệu bổ sung
-Liệt kê mô tả ... lỗi tranh chấp (….)
-Tổng hợp báo cáo lần 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mô tả chức năng hệ thống
-Ràng buộc dữ liệu bổ sung
-Liệt kê mô tả ... lỗi tranh chấp (….)
-Tổng hợp báo cáo lần 3
-</t>
-  </si>
-  <si>
-    <t>Mô tả chức năng hệ thống
-Lược đồ thực thể
-Ràng buộc dữ liệu bổ sung
-Liệt kê mô tả ... lỗi tranh chấp (….)
-Tổng hợp báo cáo lần 3</t>
   </si>
   <si>
     <t>Không có</t>
@@ -131,6 +93,46 @@
   <si>
     <t>Victim: SP_LOAD_DSGV_CUNG_GVQL
 Cause: SP_UPDATEGVQL</t>
+  </si>
+  <si>
+    <t>(NGUOIDUNG) Cập nhật thông tin</t>
+  </si>
+  <si>
+    <t>sp_DangNhap
+sp_CapNhatThongTin</t>
+  </si>
+  <si>
+    <t>(NGUOIDUNG) Thêm người dùng
+(BOMON) Xóa bộ môn</t>
+  </si>
+  <si>
+    <t>sp_TaoTaiKhoan
+sp_XoaBoMon</t>
+  </si>
+  <si>
+    <t>(BOMON)Xóa bộ môn
+(NGUOIDUNG) Thêm người dùng</t>
+  </si>
+  <si>
+    <t>sp_XoaBoMon
+sp_TaoTaiKhoan</t>
+  </si>
+  <si>
+    <t>(NGUOIDUNG) CẬP NHẬT THÔNG TIN NGƯỜI DÙNG
+(NGUOIDUNG) THAY ĐỔI GVQL</t>
+  </si>
+  <si>
+    <t>sp_CapNhatThongTin
+sp_ThayDoiGVQL</t>
+  </si>
+  <si>
+    <t>(NGUOIDUNG)
+Cập nhật thông tin
+(NGUOIDUNG)Xóa tài khoản</t>
+  </si>
+  <si>
+    <t>sp_CapNhatThongTin
+sp_XoaTaiKhoan</t>
   </si>
   <si>
     <r>
@@ -140,7 +142,111 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Giao diện:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Quản lý đề thi
+2. Quản lý câu hỏi</t>
+    </r>
+  </si>
+  <si>
+    <t>Quản lý câu hỏi</t>
+  </si>
+  <si>
+    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
+sp_LayDanhSachCauTraLoiTheoCauHoi_DEMO</t>
+  </si>
+  <si>
+    <t>sp_LayDanhSachCauHoiTheoMucDO_DEMO
+sp_CapNhatCauHoi_DEMO</t>
+  </si>
+  <si>
+    <t>Quản lý câu hỏi
+Quản lý đề thi</t>
+  </si>
+  <si>
+    <t>sp_LayDanhSachCauHoiTheoDeThi_DEMO
+sp_ThemCauHoiVaoBoDeThi_DEMO</t>
+  </si>
+  <si>
+    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
+sp_XoaCauTraLoi_DEMO</t>
+  </si>
+  <si>
+    <t>sp_CapNhatCauTraLoiSangCauHoiKhac_DEMO
+sp_XoaCauTraLoiTheoCauHoi_DEMO</t>
+  </si>
+  <si>
+    <t>sp_CapNhatMonHoc
+sp_LayMonHoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp_XoaCauHoi
+sp_Laydanhsachcauhoi </t>
+  </si>
+  <si>
+    <t>sp_CapNhatCauHoi
+sp_ThayDoiMonHoc</t>
+  </si>
+  <si>
+    <t>sp_Soluongcauhoicuabomon
+sp_ThemCauHoi</t>
+  </si>
+  <si>
+    <t>sp_CapNhatCauHoi
+sp_XoaCauHoi</t>
+  </si>
+  <si>
+    <t>Cài đặt DB</t>
+  </si>
+  <si>
+    <t>sp_XoaMonHoc
+sp_CapNhatMonHoc</t>
+  </si>
+  <si>
+    <t>sp_LayMonHoc
+sp_ThemMonHoc</t>
+  </si>
+  <si>
+    <t>Mô tả chức năng hệ thống
+Ràng buộc dữ liệu bổ sung
+Liệt kê mô tả 05 lỗi tranh chấp (ERR11~ERR15)
+Tổng hợp báo cáo lần 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mô tả chức năng hệ thống
+Ràng buộc dữ liệu bổ sung
+Liệt kê mô tả 02 lỗi tranh chấp (ERR16~ERR17)
+Tổng hợp báo cáo lần 3
+</t>
+  </si>
+  <si>
+    <t>Mô tả chức năng hệ thống
+Ràng buộc dữ liệu bổ sung
+Liệt kê mô tả 04 lỗi tranh chấp (ERR21~ERR24)
+Tổng hợp báo cáo lần 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -150,26 +256,26 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Tranh chấp ERR05 -&gt; ERR10
+      <t xml:space="preserve"> Tranh chấp 
 Cài đặt Store Procedure:
-1. sp_CapNhatThongTin
-2. sp_CapNhatTrangThai
-3. sp_CapQuyenQuanLy
-4. sp_LayDanhSachBoMon
-5. sp_LayDanhSachGiaoVienQuanLy
-6. sp_LayDanhSachNguoiDung
-7. sp_LayNguoiDung
-8. sp_TaoTaiKhoan
-9. sp_ThayDoiGVQL
-10. sp_ThemBoMon
-11. sp_XoaBoMon
-12. sp_XoaTaiKhoan
+1. sp_CapNhatCauHoi
+2. sp_Laydanhsachcauhoi
+3. sp_PhanLoaiCauhoi
+4. sp_Soluongcauhoicuabomon
+5. sp_Soluongcautraloicuacauhoi 
+6. sp_ThayDoiMonHoc
+7. sp_ThemCauHoi
+8. sp_TimKiemCauHoi
+9. sp_XoaCauHoi
+10.sp_XuatDanhSachCauHoi
 </t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -177,79 +283,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Giao diện:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1. Xem danh sách người dùng
-2. Thêm người dùng 
-3. Chỉnh sửa thông tin người dùng
-4. Xóa người dùng
-5. Thay đổi GVQL của GV
-6. Thêm bộ môn
-7. Xóa bộ môn</t>
-    </r>
-  </si>
-  <si>
-    <t>(NGUOIDUNG) Cập nhật thông tin</t>
-  </si>
-  <si>
-    <t>sp_DangNhap
-sp_CapNhatThongTin</t>
-  </si>
-  <si>
-    <t>(NGUOIDUNG) Thêm người dùng
-(BOMON) Xóa bộ môn</t>
-  </si>
-  <si>
-    <t>sp_TaoTaiKhoan
-sp_XoaBoMon</t>
-  </si>
-  <si>
-    <t>(BOMON)Xóa bộ môn
-(NGUOIDUNG) Thêm người dùng</t>
-  </si>
-  <si>
-    <t>sp_XoaBoMon
-sp_TaoTaiKhoan</t>
-  </si>
-  <si>
-    <t>(NGUOIDUNG) CẬP NHẬT THÔNG TIN NGƯỜI DÙNG
-(NGUOIDUNG) THAY ĐỔI GVQL</t>
-  </si>
-  <si>
-    <t>sp_CapNhatThongTin
-sp_ThayDoiGVQL</t>
-  </si>
-  <si>
-    <t>(NGUOIDUNG)
-Cập nhật thông tin
-(NGUOIDUNG)Xóa tài khoản</t>
-  </si>
-  <si>
-    <t>sp_CapNhatThongTin
-sp_XoaTaiKhoan</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -259,11 +293,11 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Tranh chấp ERR05 -&gt; ERR10
+      <t>Tranh chấp
 Cài đặt Store Procedure:
 1. sp_CapNhatBoDeThi
 2. sp_CapNhatCauHoi
@@ -296,7 +330,87 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Giao diện</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Thêm môn học
+2. Tìm kiếm môn học
+3. Cập nhật môn học</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tranh chấp 
+Cài đặt Store Procedure:
+1. sp_CapNhatThongTin
+2. sp_CapNhatTrangThai
+3. sp_CapQuyenQuanLy
+4. sp_LayDanhSachBoMon
+5. sp_LayDanhSachGiaoVienQuanLy
+6. sp_LayDanhSachNguoiDung
+7. sp_LayNguoiDung
+8. sp_TaoTaiKhoan
+9. sp_ThayDoiGVQL
+10. sp_ThemBoMon
+11. sp_XoaBoMon
+12. sp_XoaTaiKhoan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -306,93 +420,87 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-1. Quản lý đề thi
-2. Quản lý câu hỏi</t>
+1. Xem danh sách người dùng
+2. Thêm người dùng 
+3. Chỉnh sửa thông tin người dùng
+4. Xóa người dùng
+5. Thay đổi GVQL của GV
+6. Thêm bộ môn
+7. Xóa bộ môn</t>
     </r>
   </si>
   <si>
-    <t>Quản lý câu hỏi</t>
-  </si>
-  <si>
-    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
-sp_LayDanhSachCauTraLoiTheoCauHoi_DEMO</t>
-  </si>
-  <si>
-    <t>sp_LayDanhSachCauHoiTheoMucDO_DEMO
-sp_CapNhatCauHoi_DEMO</t>
-  </si>
-  <si>
-    <t>Quản lý câu hỏi
-Quản lý đề thi</t>
-  </si>
-  <si>
-    <t>sp_LayDanhSachCauHoiTheoDeThi_DEMO
-sp_ThemCauHoiVaoBoDeThi_DEMO</t>
-  </si>
-  <si>
-    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
-sp_XoaCauTraLoi_DEMO</t>
-  </si>
-  <si>
-    <t>sp_CapNhatCauTraLoiSangCauHoiKhac_DEMO
-sp_XoaCauTraLoiTheoCauHoi_DEMO</t>
-  </si>
-  <si>
-    <t>Thêm môn học</t>
-  </si>
-  <si>
-    <t>sp_CapNhatMonHoc
-sp_LayMonHoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database: Tranh chấp ERR11 -&gt; ERR15
-Cài đặt Store Procedure:
-1. sp_CapNhatCauHoi
-2. sp_Laydanhsachcauhoi
-3. sp_PhanLoaiCauhoi
-4. sp_Soluongcauhoicuabomon
-5. sp_Soluongcautraloicuacauhoi 
-6. sp_ThayDoiMonHoc
-7. sp_ThemCauHoi
-8. sp_TimKiemCauHoi
-9. sp_XoaCauHoi
-10.sp_XuatDanhSachCauHoi
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Database: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tranh chấp
+1. sp_CapNhatMonHoc
+2. sp_ThemMonHoc
+3. sp_LayMonHoc
+4. sp_XoaMonHoc</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sp_XoaCauHoi
-sp_Laydanhsachcauhoi </t>
-  </si>
-  <si>
-    <t>sp_CapNhatCauHoi
-sp_ThayDoiMonHoc</t>
-  </si>
-  <si>
-    <t>sp_Soluongcauhoicuabomon
-sp_ThemCauHoi</t>
-  </si>
-  <si>
-    <t>sp_CapNhatCauHoi
-sp_XoaCauHoi</t>
-  </si>
-  <si>
-    <t>Cài đặt DB</t>
+    </r>
+  </si>
+  <si>
+    <t>Mô tả chức năng hệ thống
+Lược đồ kết hợp
+Ràng buộc dữ liệu bổ sung
+Liệt kê mô tả 5 lỗi tranh chấp (ERR06~ERR10)
+Tổng hợp báo cáo lần 2</t>
+  </si>
+  <si>
+    <t>Mô tả chức năng hệ thống
+Lược đồ thực thể
+Ràng buộc dữ liệu bổ sung
+Liệt kê mô tả 05 lỗi tranh chấp (ERR01~ERR05)
+Tổng hợp báo cáo lần 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -400,7 +508,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -408,14 +516,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -423,14 +531,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -440,7 +548,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -638,6 +746,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,12 +797,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -973,125 +1081,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.9140625" customWidth="1"/>
+    <col min="6" max="6" width="21.9140625" customWidth="1"/>
     <col min="7" max="16" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="14" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="17"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="25" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="12" t="s">
+      <c r="N3" s="27"/>
+      <c r="O3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="24" t="s">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="24" t="s">
+      <c r="R3" s="25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1122,247 +1230,251 @@
       <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
     </row>
-    <row r="5" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>1642050</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="H5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="M5" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="210" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>1642067</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="10" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="182" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1642071</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="10" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="F7" s="10"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="112" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>1642076</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="10" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F8" s="10"/>
       <c r="G8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="11">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>1642084</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="O9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="11">
@@ -1371,6 +1483,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="G2:R2"/>
@@ -1387,7 +1500,6 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
update bảng đánh giá
</commit_message>
<xml_diff>
--- a/Document/Bang_danh_gia.xlsx
+++ b/Document/Bang_danh_gia.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="32660" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="465" windowWidth="32655" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>BẢNG ĐÁNH GIÁ CÁ NHÂN - NHÓM 5</t>
   </si>
@@ -142,7 +142,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -152,7 +152,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -209,9 +209,6 @@
 sp_XoaCauHoi</t>
   </si>
   <si>
-    <t>Cài đặt DB</t>
-  </si>
-  <si>
     <t>sp_XoaMonHoc
 sp_CapNhatMonHoc</t>
   </si>
@@ -246,7 +243,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -256,7 +253,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -283,7 +280,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -293,7 +290,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -330,7 +327,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -340,7 +337,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -358,7 +355,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -368,7 +365,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -395,7 +392,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -410,7 +407,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -420,7 +417,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -442,7 +439,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -452,7 +449,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -469,7 +466,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -491,16 +488,33 @@
 Liệt kê mô tả 05 lỗi tranh chấp (ERR01~ERR05)
 Tổng hợp báo cáo lần 3</t>
   </si>
+  <si>
+    <t>Database: Tranh chấp 
+Cài đặt Store Procedure:
+1. sp_GVQLCAPQUYEN
+2. sp_LayDanhSachGV</t>
+  </si>
+  <si>
+    <t>Victim: sp_UpdateToanQuyenGV1
+Cause: sp_UpdateToanQuyenGV2</t>
+  </si>
+  <si>
+    <t>Victim: sp_UpdateToanQuyenGV2_Deadlock
+Cause: sp_UpdateToanQuyenGV1_Deadlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giáo viên quản lý </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -508,7 +522,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -516,14 +530,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -531,14 +545,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -548,7 +562,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -746,6 +760,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -785,9 +802,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,7 +813,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1081,125 +1095,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="31.9140625" customWidth="1"/>
-    <col min="6" max="6" width="21.9140625" customWidth="1"/>
-    <col min="7" max="16" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1" ht="23" x14ac:dyDescent="0.5">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="15" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="28"/>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="23"/>
+      <c r="L3" s="24"/>
       <c r="M3" s="26" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="27"/>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="25" t="s">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="25" t="s">
+      <c r="R3" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1230,27 +1244,27 @@
       <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:18" ht="200" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>1642050</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>19</v>
@@ -1268,7 +1282,7 @@
         <v>19</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>19</v>
@@ -1280,29 +1294,29 @@
         <v>19</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="210" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>1642067</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>22</v>
@@ -1339,19 +1353,19 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="182" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1642071</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
@@ -1379,29 +1393,29 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="112" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>1642076</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="9" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>21</v>
@@ -1413,35 +1427,35 @@
         <v>19</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>1642084</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>32</v>
@@ -1483,11 +1497,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="A1:R1"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
@@ -1497,9 +1506,14 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="G2:R2"/>
+    <mergeCell ref="A1:R1"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Doc & implement feature
</commit_message>
<xml_diff>
--- a/Document/Bang_danh_gia.xlsx
+++ b/Document/Bang_danh_gia.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="465" windowWidth="32655" windowHeight="20535"/>
+    <workbookView xWindow="950" yWindow="470" windowWidth="32660" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>BẢNG ĐÁNH GIÁ CÁ NHÂN - NHÓM 5</t>
   </si>
@@ -142,7 +142,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -152,7 +152,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -243,7 +243,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -253,7 +253,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -280,54 +280,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Database: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tranh chấp
-Cài đặt Store Procedure:
-1. sp_CapNhatBoDeThi
-2. sp_CapNhatCauHoi
-3. sp_CapNhatCauHoiSangBoDeThiKhac
-4.sp_CapNhatCauTraLoi
-5. sp_DangNhap
-6. sp_DiChuyenCauHoiRaKhoiDeThi
-7.sp_LayDanhSachBoDeThi
-8. sp_LayDanhSachCauHoi
-9. sp_LayDanhSachCauHoiTheoDeThi
-10. sp_LayDanhSachCauHoiTheoMonHocChuaCoTrongDeThi
-11. sp_LayDanhSachCauHoiTheoMucDo
-12. sp_LayDanhSachCauTraLoiTheoCauHoi
-13. sp_LayDanhSachMonHoc
-14. sp_TaoBoDeThi
-15. sp_ThemCauHoi
-16. sp_ThemCauHoiVaoBoDeThi
-17. sp_ThemCauTraLoiVaoCauHoi
-18. sp_TimKiemBoDeThi
-19. sp_TimKiemTatCaCauHoiTheoBoDeThi
-20. sp_XoaCauHoiTrongBodeThi
-21. sp_XoaCauTraLoi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -337,7 +290,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -355,7 +308,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -365,7 +318,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -392,7 +345,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -407,7 +360,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -417,7 +370,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -439,7 +392,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -449,7 +402,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -466,7 +419,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -505,16 +458,83 @@
   <si>
     <t xml:space="preserve">Giáo viên quản lý </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Database: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tranh chấp
+Cài đặt Store Procedure:
+1. sp_CapNhatBoDeThi
+2. sp_CapNhatCauHoi
+3. sp_CapNhatCauHoiSangBoDeThiKhac
+4.sp_CapNhatCauTraLoi
+5. sp_DangNhap
+6. sp_DiChuyenCauHoiRaKhoiDeThi
+7.sp_LayDanhSachBoDeThi
+8. sp_LayDanhSachCauHoi
+9. sp_LayDanhSachCauHoiTheoDeThi
+10. sp_LayDanhSachCauHoiTheoMonHoc ChuaCoTrongDeThi
+11. sp_LayDanhSachCauHoiTheoMucDo
+12. sp_LayDanhSachCauTraLoiTheoCauHoi
+13. sp_LayDanhSachMonHoc
+14. sp_TaoBoDeThi
+15. sp_ThemCauHoi
+16. sp_ThemCauHoiVaoBoDeThi
+17. sp_ThemCauTraLoiVaoCauHoi
+18. sp_TimKiemBoDeThi
+19. sp_TimKiemTatCaCauHoiTheoBoDeThi
+20. sp_XoaCauHoiTrongBodeThi
+21. sp_XoaCauTraLoi</t>
+    </r>
+  </si>
+  <si>
+    <t>(MONHOC)
+Cập nhật môn học
+Lấy danh sách môn học</t>
+  </si>
+  <si>
+    <t>(MONHOC)
+Lấy sanh sách môn học
+Cập nhật môn học</t>
+  </si>
+  <si>
+    <t>(MONHOC)
+Lấy danh sách môn học
+Thêm môn học</t>
+  </si>
+  <si>
+    <t>(MONHOC)
+Cập nhật môn học
+Xóa môn học</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -522,7 +542,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -530,29 +550,21 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -562,7 +574,15 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -750,7 +770,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,30 +780,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -802,18 +798,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1095,125 +1115,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="16" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.25" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="16" width="19.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.6">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="16" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="25"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="23" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="26" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="27"/>
-      <c r="O3" s="14" t="s">
+      <c r="N3" s="28"/>
+      <c r="O3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="12" t="s">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1244,42 +1264,42 @@
       <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
     </row>
-    <row r="5" spans="1:18" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="200.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>1642050</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>46</v>
@@ -1291,32 +1311,32 @@
         <v>19</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>45</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="11">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="240" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="225.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>1642067</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>22</v>
@@ -1353,14 +1373,14 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="182" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1642071</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="10" t="s">
         <v>47</v>
       </c>
@@ -1393,29 +1413,29 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="198.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>1642076</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>21</v>
@@ -1427,35 +1447,35 @@
         <v>19</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="336" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>1642084</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>32</v>
@@ -1497,6 +1517,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="G2:R2"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
@@ -1507,15 +1534,8 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify Dirty Read ( GUI & Script )
</commit_message>
<xml_diff>
--- a/Document/Bang_danh_gia.xlsx
+++ b/Document/Bang_danh_gia.xlsx
@@ -1,19 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="950" yWindow="470" windowWidth="32660" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="465" windowWidth="32655" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -142,7 +139,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -152,7 +149,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -165,10 +162,6 @@
     <t>Quản lý câu hỏi</t>
   </si>
   <si>
-    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
-sp_LayDanhSachCauTraLoiTheoCauHoi_DEMO</t>
-  </si>
-  <si>
     <t>sp_LayDanhSachCauHoiTheoMucDO_DEMO
 sp_CapNhatCauHoi_DEMO</t>
   </si>
@@ -243,7 +236,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -253,7 +246,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -280,7 +273,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -290,7 +283,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -308,7 +301,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -318,7 +311,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -345,7 +338,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -360,7 +353,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -370,7 +363,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -392,7 +385,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -402,7 +395,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -419,7 +412,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -466,7 +459,7 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -476,7 +469,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -525,16 +518,20 @@
 Cập nhật môn học
 Xóa môn học</t>
   </si>
+  <si>
+    <t>sp_ThemCauTraLoiVaoCauHoi_DEMO
+sp_LayDanhSachCauHoi_DEMO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -542,7 +539,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -550,21 +547,21 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -574,7 +571,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -582,7 +579,7 @@
       <b/>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -780,6 +777,36 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -801,39 +828,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -896,7 +893,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -931,7 +928,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1108,132 +1105,132 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22.75" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
-    <col min="7" max="16" width="19.58203125" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="16" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.6">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="23" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="25"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="15" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16" t="s">
+      <c r="J3" s="25"/>
+      <c r="K3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="27" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="28"/>
-      <c r="O3" s="21" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1264,45 +1261,45 @@
       <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:18" ht="200.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>1642050</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="L5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>19</v>
@@ -1311,32 +1308,32 @@
         <v>19</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="11">
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="225.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="225.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <v>1642067</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>22</v>
@@ -1373,69 +1370,69 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="182" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1642071</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="198.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>1642076</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>21</v>
@@ -1447,35 +1444,35 @@
         <v>19</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="336" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="360" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>1642084</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>32</v>
@@ -1484,31 +1481,31 @@
         <v>33</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="J9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="11">
@@ -1517,13 +1514,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
@@ -1534,6 +1524,13 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="G2:R2"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="58" orientation="landscape" r:id="rId1"/>

</xml_diff>